<commit_message>
List of user stories/points
Completed list of user stories.
Added story point values.
</commit_message>
<xml_diff>
--- a/sprint_2/User Stories and Points.xlsx
+++ b/sprint_2/User Stories and Points.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0cb1501512501fd7/Documents/School/Winter 2022/SOEN 341/Sprint 2 files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5a8631b9265da2/Documents/GitHub/GENERALs-soen341project2022/sprint_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{3E2D162C-5AB3-4844-8071-1C5539583212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CF76FD3-1509-4A0D-AF1F-C65BDF2DC51F}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{3E2D162C-5AB3-4844-8071-1C5539583212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{596394C0-002B-496E-8A60-CC9A73F19E15}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="2250" windowWidth="28800" windowHeight="15435" xr2:uid="{EDC6FAB9-E1FB-43EF-B5FF-9A15F1E94E5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{EDC6FAB9-E1FB-43EF-B5FF-9A15F1E94E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>User Story</t>
   </si>
   <si>
     <t>Story Points</t>
-  </si>
-  <si>
-    <t>Reasoning</t>
   </si>
   <si>
     <t>As a customer, I want to be able to change my home address, because I recently moved to a new house.</t>
@@ -52,7 +49,13 @@
     <t>As a customer, I want to be able to find groupings of items easily, because I don't want to search the entire catalogue of items on the website for one thing.</t>
   </si>
   <si>
-    <t>As a customer, I want to be able to change my username, email and password, because I'm concerned about my previous information being compromised</t>
+    <t xml:space="preserve">As a customer, I want to be able to find items that fit my budget. </t>
+  </si>
+  <si>
+    <t>As a customer, I want to be able to change my username, email and password, because I'm concerned about my previous information being compromised.</t>
+  </si>
+  <si>
+    <t>As a customer, I want to have a Wish list that have all my favorite items, because I want it to be easy to locate them later when it is the appropriate time to buy them.</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -91,21 +94,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -120,48 +108,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -205,29 +156,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -244,7 +212,14 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -254,6 +229,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -275,56 +257,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -341,12 +273,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C5D7A91-F8B9-481A-B836-78898DEAF58F}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:C8" xr:uid="{7C5D7A91-F8B9-481A-B836-78898DEAF58F}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FCBFED7C-4F63-42D6-AA8C-69FE022A397D}" name="User Story" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E01EBF91-F674-44A0-83B8-544CF72A8EDB}" name="Story Points" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{7CE13C1D-3816-4C5C-86C7-B4F06B5331D0}" name="Reasoning" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C5D7A91-F8B9-481A-B836-78898DEAF58F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="A1:B6" xr:uid="{7C5D7A91-F8B9-481A-B836-78898DEAF58F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FCBFED7C-4F63-42D6-AA8C-69FE022A397D}" name="User Story" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E01EBF91-F674-44A0-83B8-544CF72A8EDB}" name="Story Points" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -649,70 +580,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D58DF4-A59B-45F2-A3D9-83F847BE7559}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="94.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="94.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="31.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="C15" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>